<commit_message>
Revised Cedar Grove Draft
</commit_message>
<xml_diff>
--- a/Budgets/Cedar Grove 2017 Budget draft 1.xlsx
+++ b/Budgets/Cedar Grove 2017 Budget draft 1.xlsx
@@ -1585,9 +1585,6 @@
     <t> CAM- LIGHTING</t>
   </si>
   <si>
-    <t>$75K? LED Retrofit Parking Lot - Potential Vendor: YESCO, BROADWAY LIGHTING</t>
-  </si>
-  <si>
     <t>reduced by 30% due to CRS SF increase</t>
   </si>
   <si>
@@ -1808,6 +1805,9 @@
   </si>
   <si>
     <t>Vacant spaces</t>
+  </si>
+  <si>
+    <t>$40K LED Retrofit Parking Lot - Potential Vendor: YESCO, BROADWAY LIGHTING</t>
   </si>
 </sst>
 </file>
@@ -3070,6 +3070,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="40" fontId="19" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3093,9 +3096,6 @@
     </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="44" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="40" fontId="19" fillId="37" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4174,44 +4174,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="218" t="s">
+      <c r="A1" s="219" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="218"/>
-      <c r="C1" s="218"/>
-      <c r="D1" s="218"/>
-      <c r="E1" s="218"/>
-      <c r="F1" s="218"/>
-      <c r="G1" s="218"/>
+      <c r="B1" s="219"/>
+      <c r="C1" s="219"/>
+      <c r="D1" s="219"/>
+      <c r="E1" s="219"/>
+      <c r="F1" s="219"/>
+      <c r="G1" s="219"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="219" t="s">
+      <c r="A2" s="220" t="s">
         <v>195</v>
       </c>
-      <c r="B2" s="219"/>
-      <c r="C2" s="219"/>
-      <c r="D2" s="219"/>
-      <c r="E2" s="219"/>
-      <c r="F2" s="219"/>
-      <c r="G2" s="219"/>
+      <c r="B2" s="220"/>
+      <c r="C2" s="220"/>
+      <c r="D2" s="220"/>
+      <c r="E2" s="220"/>
+      <c r="F2" s="220"/>
+      <c r="G2" s="220"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="218"/>
-      <c r="B3" s="218"/>
-      <c r="C3" s="218"/>
-      <c r="D3" s="218"/>
-      <c r="E3" s="218"/>
-      <c r="F3" s="218"/>
-      <c r="G3" s="218"/>
+      <c r="A3" s="219"/>
+      <c r="B3" s="219"/>
+      <c r="C3" s="219"/>
+      <c r="D3" s="219"/>
+      <c r="E3" s="219"/>
+      <c r="F3" s="219"/>
+      <c r="G3" s="219"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="218"/>
-      <c r="B4" s="218"/>
-      <c r="C4" s="218"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="218"/>
-      <c r="F4" s="218"/>
-      <c r="G4" s="218"/>
+      <c r="A4" s="219"/>
+      <c r="B4" s="219"/>
+      <c r="C4" s="219"/>
+      <c r="D4" s="219"/>
+      <c r="E4" s="219"/>
+      <c r="F4" s="219"/>
+      <c r="G4" s="219"/>
     </row>
     <row r="5" spans="1:9" s="11" customFormat="1" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
@@ -5734,13 +5734,13 @@
       <c r="I97" s="1"/>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A98" s="217"/>
-      <c r="B98" s="217"/>
-      <c r="C98" s="217"/>
-      <c r="D98" s="217"/>
-      <c r="E98" s="217"/>
-      <c r="F98" s="217"/>
-      <c r="G98" s="217"/>
+      <c r="A98" s="218"/>
+      <c r="B98" s="218"/>
+      <c r="C98" s="218"/>
+      <c r="D98" s="218"/>
+      <c r="E98" s="218"/>
+      <c r="F98" s="218"/>
+      <c r="G98" s="218"/>
       <c r="I98" s="1"/>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -5866,13 +5866,13 @@
       <c r="I105" s="1"/>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A106" s="217"/>
-      <c r="B106" s="217"/>
-      <c r="C106" s="217"/>
-      <c r="D106" s="217"/>
-      <c r="E106" s="217"/>
-      <c r="F106" s="217"/>
-      <c r="G106" s="217"/>
+      <c r="A106" s="218"/>
+      <c r="B106" s="218"/>
+      <c r="C106" s="218"/>
+      <c r="D106" s="218"/>
+      <c r="E106" s="218"/>
+      <c r="F106" s="218"/>
+      <c r="G106" s="218"/>
       <c r="I106" s="1"/>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -6150,12 +6150,12 @@
         <v>9138488.0199999996</v>
       </c>
       <c r="N3" s="121" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="204" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="B4" s="210">
         <v>2.1999999999999999E-2</v>
@@ -6195,7 +6195,7 @@
         <v>9126930.4699999988</v>
       </c>
       <c r="N4" s="204" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O4" s="214">
         <f>'[2]Base Rent 2016'!C8</f>
@@ -6244,7 +6244,7 @@
         <v>9115327.1699999981</v>
       </c>
       <c r="N5" s="204" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O5" s="88">
         <v>45</v>
@@ -6322,7 +6322,7 @@
         <v>9091982.5999999978</v>
       </c>
       <c r="N7" s="204" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O7" s="103">
         <f>(O$4*O$5)/4</f>
@@ -6365,7 +6365,7 @@
         <v>9080240.9699999969</v>
       </c>
       <c r="N8" s="204" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O8" s="103">
         <f t="shared" ref="O8:O10" si="7">(O$4*O$5)/4</f>
@@ -6414,7 +6414,7 @@
         <v>9068452.8599999975</v>
       </c>
       <c r="N9" s="204" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O9" s="103">
         <f t="shared" si="7"/>
@@ -6463,7 +6463,7 @@
         <v>9056618.089999998</v>
       </c>
       <c r="N10" s="204" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O10" s="103">
         <f t="shared" si="7"/>
@@ -6591,7 +6591,7 @@
         <v>9020831.9499999993</v>
       </c>
       <c r="N13" s="121" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
@@ -6630,7 +6630,7 @@
         <v>9008808.6799999997</v>
       </c>
       <c r="N14" s="204" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O14" s="214">
         <f>'[2]Base Rent 2016'!C9</f>
@@ -6674,7 +6674,7 @@
         <v>8996737.8200000003</v>
       </c>
       <c r="N15" s="204" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O15" s="88">
         <v>50</v>
@@ -6753,7 +6753,7 @@
         <v>8972452.5700000003</v>
       </c>
       <c r="N17" s="204" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O17" s="103">
         <f>(O$14*O$15)/4</f>
@@ -6796,7 +6796,7 @@
         <v>8960237.8000000007</v>
       </c>
       <c r="N18" s="204" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O18" s="103">
         <f t="shared" ref="O18:O20" si="8">(O$14*O$15)/4</f>
@@ -6839,7 +6839,7 @@
         <v>8947974.6800000016</v>
       </c>
       <c r="N19" s="204" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O19" s="103">
         <f t="shared" si="8"/>
@@ -6882,7 +6882,7 @@
         <v>8935663.0200000014</v>
       </c>
       <c r="N20" s="204" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O20" s="103">
         <f t="shared" si="8"/>
@@ -6998,7 +6998,7 @@
         <v>8898434.8600000013</v>
       </c>
       <c r="N23" s="121" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="24" spans="4:15" x14ac:dyDescent="0.25">
@@ -7037,7 +7037,7 @@
         <v>8885927.1000000015</v>
       </c>
       <c r="N24" s="204" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O24" s="214">
         <f xml:space="preserve"> '[2]Base Rent 2016'!C10</f>
@@ -7080,7 +7080,7 @@
         <v>8873369.8300000019</v>
       </c>
       <c r="N25" s="204" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O25" s="88">
         <v>25</v>
@@ -7158,7 +7158,7 @@
         <v>8848105.9800000004</v>
       </c>
       <c r="N27" s="204" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O27" s="103">
         <f>(O$24*O$25)/4</f>
@@ -7201,7 +7201,7 @@
         <v>8835399</v>
       </c>
       <c r="N28" s="204" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O28" s="103">
         <f t="shared" ref="O28:O30" si="9">(O$24*O$25)/4</f>
@@ -7244,7 +7244,7 @@
         <v>8822641.7200000007</v>
       </c>
       <c r="N29" s="204" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O29" s="103">
         <f t="shared" si="9"/>
@@ -7287,7 +7287,7 @@
         <v>8809833.9500000011</v>
       </c>
       <c r="N30" s="204" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O30" s="103">
         <f t="shared" si="9"/>
@@ -7402,7 +7402,7 @@
         <v>8771105.6400000006</v>
       </c>
       <c r="N33" s="121" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="34" spans="4:15" x14ac:dyDescent="0.25">
@@ -7441,7 +7441,7 @@
         <v>8758093.870000001</v>
       </c>
       <c r="N34" s="204" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="O34" s="214">
         <f>'[2]Base Rent 2016'!C11</f>
@@ -7484,7 +7484,7 @@
         <v>8745030.5900000017</v>
       </c>
       <c r="N35" s="204" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="O35" s="88">
         <v>25</v>
@@ -7562,7 +7562,7 @@
         <v>8718748.7100000009</v>
       </c>
       <c r="N37" s="204" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="O37" s="103">
         <f>(O$34*O$35)/4</f>
@@ -7605,7 +7605,7 @@
         <v>8705529.6900000013</v>
       </c>
       <c r="N38" s="204" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O38" s="103">
         <f t="shared" ref="O38:O40" si="10">(O$34*O$35)/4</f>
@@ -7648,7 +7648,7 @@
         <v>8692258.3500000015</v>
       </c>
       <c r="N39" s="204" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O39" s="103">
         <f t="shared" si="10"/>
@@ -7691,7 +7691,7 @@
         <v>8678934.4800000023</v>
       </c>
       <c r="N40" s="204" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="O40" s="103">
         <f t="shared" si="10"/>
@@ -13693,15 +13693,15 @@
       <c r="D21" s="89"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="224" t="s">
+      <c r="A22" s="225" t="s">
         <v>339</v>
       </c>
-      <c r="B22" s="224"/>
+      <c r="B22" s="225"/>
       <c r="D22" s="89"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="224"/>
-      <c r="B23" s="224"/>
+      <c r="A23" s="225"/>
+      <c r="B23" s="225"/>
       <c r="D23" s="89"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -18305,9 +18305,9 @@
   </sheetPr>
   <dimension ref="A1:AE243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S118" sqref="S118"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="70" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D206" sqref="D206"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -18328,47 +18328,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="19.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="220" t="s">
-        <v>511</v>
-      </c>
-      <c r="B1" s="220"/>
-      <c r="C1" s="220"/>
-      <c r="D1" s="220"/>
-      <c r="E1" s="220"/>
-      <c r="F1" s="220"/>
-      <c r="G1" s="220"/>
-      <c r="H1" s="220"/>
-      <c r="I1" s="220"/>
-      <c r="J1" s="220"/>
-      <c r="K1" s="220"/>
-      <c r="L1" s="220"/>
-      <c r="M1" s="220"/>
-      <c r="N1" s="220"/>
-      <c r="O1" s="220"/>
-      <c r="P1" s="220"/>
-      <c r="Q1" s="220"/>
+      <c r="A1" s="221" t="s">
+        <v>510</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="221"/>
+      <c r="I1" s="221"/>
+      <c r="J1" s="221"/>
+      <c r="K1" s="221"/>
+      <c r="L1" s="221"/>
+      <c r="M1" s="221"/>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="221"/>
       <c r="R1" s="181"/>
     </row>
     <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="221" t="s">
+      <c r="A2" s="222" t="s">
         <v>392</v>
       </c>
-      <c r="B2" s="221"/>
-      <c r="C2" s="221"/>
-      <c r="D2" s="221"/>
-      <c r="E2" s="221"/>
-      <c r="F2" s="221"/>
-      <c r="G2" s="221"/>
-      <c r="H2" s="221"/>
-      <c r="I2" s="221"/>
-      <c r="J2" s="221"/>
-      <c r="K2" s="221"/>
-      <c r="L2" s="221"/>
-      <c r="M2" s="221"/>
-      <c r="N2" s="221"/>
-      <c r="O2" s="221"/>
-      <c r="P2" s="221"/>
-      <c r="Q2" s="221"/>
+      <c r="B2" s="222"/>
+      <c r="C2" s="222"/>
+      <c r="D2" s="222"/>
+      <c r="E2" s="222"/>
+      <c r="F2" s="222"/>
+      <c r="G2" s="222"/>
+      <c r="H2" s="222"/>
+      <c r="I2" s="222"/>
+      <c r="J2" s="222"/>
+      <c r="K2" s="222"/>
+      <c r="L2" s="222"/>
+      <c r="M2" s="222"/>
+      <c r="N2" s="222"/>
+      <c r="O2" s="222"/>
+      <c r="P2" s="222"/>
+      <c r="Q2" s="222"/>
       <c r="R2" s="182"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -18460,7 +18460,7 @@
         <v>0</v>
       </c>
       <c r="R5" s="183" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="S5" s="132" t="s">
         <v>203</v>
@@ -18626,10 +18626,10 @@
         <v>7.0811971744834806E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C11" s="128">
         <v>41697</v>
@@ -18695,10 +18695,10 @@
         <v>3.2776458738038715E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C12" s="128">
         <v>28035</v>
@@ -18764,10 +18764,10 @@
         <v>7.4666666666666881E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C13" s="128">
         <v>73167</v>
@@ -18833,10 +18833,10 @@
         <v>-6.5603345770077419E-6</v>
       </c>
     </row>
-    <row r="14" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="31" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C14" s="128">
         <v>80039</v>
@@ -18902,10 +18902,10 @@
         <v>-9.9951273719864559E-7</v>
       </c>
     </row>
-    <row r="15" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C15" s="128">
         <v>83503</v>
@@ -18971,10 +18971,10 @@
         <v>5.8739925511658339E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7"/>
       <c r="B16" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C16" s="128">
         <v>61500</v>
@@ -19040,10 +19040,10 @@
         <v>-2.4390243902439025E-2</v>
       </c>
     </row>
-    <row r="17" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7"/>
       <c r="B17" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C17" s="128">
         <v>48026</v>
@@ -19109,13 +19109,13 @@
         <v>-0.19910132011826914</v>
       </c>
       <c r="S17" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="18" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
       <c r="B18" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C18" s="128">
         <v>43014</v>
@@ -19181,10 +19181,10 @@
         <v>2.1120565397312746E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7"/>
       <c r="B19" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C19" s="128">
         <v>73267</v>
@@ -19250,10 +19250,10 @@
         <v>2.9998225667762977E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A20" s="7"/>
       <c r="B20" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C20" s="128">
         <v>12157</v>
@@ -19319,10 +19319,10 @@
         <v>1.2535164925557394E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7"/>
       <c r="B21" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C21" s="128">
         <v>40826</v>
@@ -19388,10 +19388,10 @@
         <v>-6.4584333512957462E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7"/>
       <c r="B22" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C22" s="128">
         <v>45000</v>
@@ -19457,10 +19457,10 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="23" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7"/>
       <c r="B23" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C23" s="128">
         <v>0</v>
@@ -19526,10 +19526,10 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C24" s="128">
         <v>51035</v>
@@ -19595,10 +19595,10 @@
         <v>2.6312138728323629E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="B25" s="125" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C25" s="128">
         <v>46247</v>
@@ -19664,10 +19664,10 @@
         <v>3.9990485869353422E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A26" s="180"/>
       <c r="B26" s="125" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C26" s="128">
         <v>37072</v>
@@ -19733,10 +19733,10 @@
         <v>2.7474104445403845E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="180"/>
       <c r="B27" s="125" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C27" s="128">
         <v>67340</v>
@@ -19802,10 +19802,10 @@
         <v>5.9400059390551166E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="180"/>
       <c r="B28" s="125" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C28" s="128">
         <v>50236</v>
@@ -19871,13 +19871,13 @@
         <v>3.0000796241738899E-2</v>
       </c>
       <c r="S28" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="29" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A29" s="180"/>
       <c r="B29" s="125" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C29" s="128">
         <v>171021</v>
@@ -19943,10 +19943,10 @@
         <v>2.2868887446570705E-2</v>
       </c>
     </row>
-    <row r="30" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A30" s="180"/>
       <c r="B30" s="125" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C30" s="128">
         <v>120957</v>
@@ -20012,10 +20012,10 @@
         <v>3.821523351273877E-3</v>
       </c>
     </row>
-    <row r="31" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="180"/>
       <c r="B31" s="125" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C31" s="128"/>
       <c r="D31" s="128">
@@ -20079,10 +20079,10 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:19" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="180"/>
       <c r="B32" s="125" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C32" s="128"/>
       <c r="D32" s="128">
@@ -20146,7 +20146,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:18" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -20436,10 +20436,10 @@
         <v>1.7852956096562837E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C40" s="128">
         <v>22651</v>
@@ -20505,10 +20505,10 @@
         <v>-1.5195797095050863E-2</v>
       </c>
     </row>
-    <row r="41" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C41" s="128">
         <v>11714</v>
@@ -20574,10 +20574,10 @@
         <v>-9.6363325934778216E-3</v>
       </c>
     </row>
-    <row r="42" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C42" s="128">
         <v>16671</v>
@@ -20643,10 +20643,10 @@
         <v>-6.7302501349649525E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="31" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C43" s="128">
         <v>30417</v>
@@ -20712,10 +20712,10 @@
         <v>-9.8905217477068784E-3</v>
       </c>
     </row>
-    <row r="44" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C44" s="128">
         <v>0</v>
@@ -20781,10 +20781,10 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C45" s="128">
         <v>18639</v>
@@ -20850,10 +20850,10 @@
         <v>-1.5708997263801667E-2</v>
       </c>
     </row>
-    <row r="46" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C46" s="128">
         <v>19415</v>
@@ -20919,10 +20919,10 @@
         <v>-2.8596446046871015E-2</v>
       </c>
     </row>
-    <row r="47" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="31" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C47" s="128">
         <v>14820</v>
@@ -20988,10 +20988,10 @@
         <v>-8.348178137651532E-3</v>
       </c>
     </row>
-    <row r="48" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C48" s="128">
         <v>26386</v>
@@ -21057,10 +21057,10 @@
         <v>0.118720533616312</v>
       </c>
     </row>
-    <row r="49" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C49" s="128">
         <v>7766</v>
@@ -21126,10 +21126,10 @@
         <v>-1.2433685294875148E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C50" s="128">
         <v>15061</v>
@@ -21195,10 +21195,10 @@
         <v>-2.3005112542328079E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C51" s="128">
         <v>16484</v>
@@ -21264,10 +21264,10 @@
         <v>-9.22106284880368E-5</v>
       </c>
     </row>
-    <row r="52" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C52" s="128">
         <v>0</v>
@@ -21333,10 +21333,10 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C53" s="128">
         <v>19415</v>
@@ -21402,10 +21402,10 @@
         <v>-2.941231006953391E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="125" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C54" s="128">
         <v>15144</v>
@@ -21471,10 +21471,10 @@
         <v>-1.0198098256735014E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A55" s="180"/>
       <c r="B55" s="125" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C55" s="128">
         <v>15015</v>
@@ -21537,10 +21537,10 @@
       </c>
       <c r="R55" s="185"/>
     </row>
-    <row r="56" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A56" s="180"/>
       <c r="B56" s="125" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C56" s="128">
         <v>13879</v>
@@ -21603,10 +21603,10 @@
       </c>
       <c r="R56" s="185"/>
     </row>
-    <row r="57" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="180"/>
       <c r="B57" s="125" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C57" s="128">
         <v>14044</v>
@@ -21669,10 +21669,10 @@
       </c>
       <c r="R57" s="185"/>
     </row>
-    <row r="58" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A58" s="180"/>
       <c r="B58" s="125" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C58" s="128">
         <v>63165</v>
@@ -21735,10 +21735,10 @@
       </c>
       <c r="R58" s="185"/>
     </row>
-    <row r="59" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A59" s="180"/>
       <c r="B59" s="125" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C59" s="128">
         <v>32741</v>
@@ -21801,10 +21801,10 @@
       </c>
       <c r="R59" s="185"/>
     </row>
-    <row r="60" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="180"/>
       <c r="B60" s="125" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C60" s="128"/>
       <c r="D60" s="128">
@@ -21865,10 +21865,10 @@
       </c>
       <c r="R60" s="185"/>
     </row>
-    <row r="61" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="180"/>
       <c r="B61" s="125" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C61" s="128"/>
       <c r="D61" s="128">
@@ -21929,7 +21929,7 @@
       </c>
       <c r="R61" s="185"/>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:18" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>17</v>
       </c>
@@ -22059,10 +22059,10 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="9" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="C64" s="128"/>
       <c r="D64" s="128">
@@ -22126,10 +22126,10 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
       <c r="B65" s="9" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="C65" s="128"/>
       <c r="D65" s="128">
@@ -22193,10 +22193,10 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
       <c r="B66" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="C66" s="128"/>
       <c r="D66" s="128">
@@ -22260,10 +22260,10 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A67" s="7"/>
       <c r="B67" s="9" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="C67" s="128"/>
       <c r="D67" s="128">
@@ -22327,10 +22327,10 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="9" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="C68" s="128"/>
       <c r="D68" s="128">
@@ -22394,10 +22394,10 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A69" s="7"/>
       <c r="B69" s="9" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="C69" s="128"/>
       <c r="D69" s="128">
@@ -22461,10 +22461,10 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="9" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="C70" s="128"/>
       <c r="D70" s="128">
@@ -22528,10 +22528,10 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="9" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="C71" s="128"/>
       <c r="D71" s="128">
@@ -22595,10 +22595,10 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="9" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="C72" s="128"/>
       <c r="D72" s="128">
@@ -22662,10 +22662,10 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C73" s="128"/>
       <c r="D73" s="128">
@@ -22729,10 +22729,10 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1"/>
       <c r="B74" s="9" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="C74" s="128"/>
       <c r="D74" s="128">
@@ -22796,10 +22796,10 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A75" s="1"/>
       <c r="B75" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="C75" s="128"/>
       <c r="D75" s="128">
@@ -22863,10 +22863,10 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="9" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="C76" s="128"/>
       <c r="D76" s="128">
@@ -22930,10 +22930,10 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1"/>
       <c r="B77" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="C77" s="128"/>
       <c r="D77" s="128">
@@ -22997,10 +22997,10 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="9" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="C78" s="128"/>
       <c r="D78" s="128">
@@ -23064,10 +23064,10 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A79" s="180"/>
       <c r="B79" s="9" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="C79" s="128"/>
       <c r="D79" s="128">
@@ -23125,10 +23125,10 @@
       <c r="Q79" s="128"/>
       <c r="R79" s="185"/>
     </row>
-    <row r="80" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A80" s="180"/>
       <c r="B80" s="9" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="C80" s="128"/>
       <c r="D80" s="128">
@@ -23186,10 +23186,10 @@
       <c r="Q80" s="128"/>
       <c r="R80" s="185"/>
     </row>
-    <row r="81" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A81" s="180"/>
       <c r="B81" s="9" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="C81" s="128"/>
       <c r="D81" s="128">
@@ -23247,10 +23247,10 @@
       <c r="Q81" s="128"/>
       <c r="R81" s="185"/>
     </row>
-    <row r="82" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A82" s="180"/>
       <c r="B82" s="9" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="C82" s="128"/>
       <c r="D82" s="128">
@@ -23308,10 +23308,10 @@
       <c r="Q82" s="128"/>
       <c r="R82" s="185"/>
     </row>
-    <row r="83" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A83" s="180"/>
       <c r="B83" s="9" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="C83" s="128"/>
       <c r="D83" s="128">
@@ -23369,10 +23369,10 @@
       <c r="Q83" s="128"/>
       <c r="R83" s="185"/>
     </row>
-    <row r="84" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A84" s="180"/>
       <c r="B84" s="9" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="C84" s="128"/>
       <c r="D84" s="128">
@@ -23430,10 +23430,10 @@
       <c r="Q84" s="128"/>
       <c r="R84" s="185"/>
     </row>
-    <row r="85" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A85" s="180"/>
       <c r="B85" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="C85" s="128"/>
       <c r="D85" s="128">
@@ -23491,7 +23491,7 @@
       <c r="Q85" s="128"/>
       <c r="R85" s="185"/>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:18" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>21</v>
       </c>
@@ -24378,7 +24378,7 @@
         <v>0.25253696723688024</v>
       </c>
       <c r="S105" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="106" spans="1:19" x14ac:dyDescent="0.25">
@@ -24394,7 +24394,7 @@
         <v>0</v>
       </c>
       <c r="E106" s="129">
-        <f t="shared" ref="E106:O107" si="16">$P$106/12</f>
+        <f t="shared" ref="E106:O106" si="16">$P$106/12</f>
         <v>0</v>
       </c>
       <c r="F106" s="129">
@@ -24451,10 +24451,10 @@
     </row>
     <row r="107" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A107" s="198" t="s">
+        <v>574</v>
+      </c>
+      <c r="B107" s="5" t="s">
         <v>575</v>
-      </c>
-      <c r="B107" s="5" t="s">
-        <v>576</v>
       </c>
       <c r="C107" s="129">
         <v>0</v>
@@ -24496,11 +24496,12 @@
         <v>300</v>
       </c>
       <c r="P107" s="128">
-        <v>0</v>
+        <f>SUM(D107:O107)</f>
+        <v>10400</v>
       </c>
       <c r="Q107" s="128">
         <f t="shared" ref="Q107" si="17">IF(C107&lt;&gt;"",P107-C107,"")</f>
-        <v>0</v>
+        <v>10400</v>
       </c>
       <c r="R107" s="185" t="str">
         <f t="shared" ref="R107" si="18">IF(C107&lt;&gt;0,Q107/C107,"")</f>
@@ -24694,7 +24695,7 @@
         <v>0</v>
       </c>
       <c r="P110" s="128">
-        <f t="shared" ref="P110:P118" si="20">C110*1.05</f>
+        <f t="shared" ref="P110:P117" si="20">C110*1.05</f>
         <v>0</v>
       </c>
       <c r="Q110" s="128" t="str">
@@ -24725,11 +24726,11 @@
       <c r="F111" s="129">
         <v>1800</v>
       </c>
-      <c r="G111" s="225">
+      <c r="G111" s="217">
         <f>1800+10000</f>
         <v>11800</v>
       </c>
-      <c r="H111" s="225">
+      <c r="H111" s="217">
         <f>1800+10000</f>
         <v>11800</v>
       </c>
@@ -24767,15 +24768,15 @@
         <v>1.009273570324575</v>
       </c>
       <c r="S111" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="112" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A112" s="188" t="s">
+        <v>571</v>
+      </c>
+      <c r="B112" s="5" t="s">
         <v>572</v>
-      </c>
-      <c r="B112" s="5" t="s">
-        <v>573</v>
       </c>
       <c r="C112" s="129">
         <v>6089</v>
@@ -24829,7 +24830,7 @@
         <v>-0.19165051732632618</v>
       </c>
       <c r="S112" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="113" spans="1:25" x14ac:dyDescent="0.25">
@@ -25078,7 +25079,7 @@
         <v>-0.15662650602409639</v>
       </c>
       <c r="S116" s="167" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="117" spans="1:25" x14ac:dyDescent="0.25">
@@ -25144,7 +25145,7 @@
         <v>0.05</v>
       </c>
       <c r="S117" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="118" spans="1:25" x14ac:dyDescent="0.25">
@@ -25159,62 +25160,63 @@
       </c>
       <c r="D118" s="129">
         <f t="shared" ref="D118:O118" si="21">$P118/12</f>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="E118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="F118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="G118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="H118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="I118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="J118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="K118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="L118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="M118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="N118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="O118" s="129">
         <f t="shared" si="21"/>
-        <v>1666.6666666666667</v>
+        <v>2220</v>
       </c>
       <c r="P118" s="203">
-        <v>20000</v>
+        <f>29600-P131</f>
+        <v>26640</v>
       </c>
       <c r="Q118" s="128">
         <f t="shared" si="12"/>
-        <v>11049</v>
+        <v>17689</v>
       </c>
       <c r="R118" s="185">
         <f t="shared" si="13"/>
-        <v>1.2343872193051055</v>
+        <v>1.9762037761144007</v>
       </c>
     </row>
     <row r="119" spans="1:25" x14ac:dyDescent="0.25">
@@ -25287,7 +25289,7 @@
         <v>0.21054353562005274</v>
       </c>
       <c r="S119" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="120" spans="1:25" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -25375,63 +25377,63 @@
       </c>
       <c r="D121" s="130">
         <f>ROUND(SUM(D104:D120),0)</f>
-        <v>24268</v>
+        <v>24821</v>
       </c>
       <c r="E121" s="130">
         <f t="shared" ref="E121:O121" si="24">ROUND(SUM(E104:E120),0)</f>
-        <v>24186</v>
+        <v>24739</v>
       </c>
       <c r="F121" s="130">
         <f t="shared" si="24"/>
-        <v>34205</v>
+        <v>34758</v>
       </c>
       <c r="G121" s="130">
         <f t="shared" si="24"/>
-        <v>35812</v>
+        <v>36365</v>
       </c>
       <c r="H121" s="130">
         <f t="shared" si="24"/>
-        <v>32748</v>
+        <v>33302</v>
       </c>
       <c r="I121" s="130">
         <f t="shared" si="24"/>
-        <v>38376</v>
+        <v>38929</v>
       </c>
       <c r="J121" s="130">
         <f t="shared" si="24"/>
-        <v>22608</v>
+        <v>23162</v>
       </c>
       <c r="K121" s="130">
         <f t="shared" si="24"/>
-        <v>32762</v>
+        <v>33316</v>
       </c>
       <c r="L121" s="130">
         <f t="shared" si="24"/>
-        <v>22537</v>
+        <v>23091</v>
       </c>
       <c r="M121" s="130">
         <f t="shared" si="24"/>
-        <v>22791</v>
+        <v>23344</v>
       </c>
       <c r="N121" s="130">
         <f t="shared" si="24"/>
-        <v>32888</v>
+        <v>33441</v>
       </c>
       <c r="O121" s="130">
         <f t="shared" si="24"/>
-        <v>23975</v>
+        <v>24528</v>
       </c>
       <c r="P121" s="130">
         <f>ROUND(SUM(P104:P120),0)</f>
-        <v>351279</v>
+        <v>368319</v>
       </c>
       <c r="Q121" s="130">
         <f t="shared" si="12"/>
-        <v>38687</v>
+        <v>55727</v>
       </c>
       <c r="R121" s="185">
         <f t="shared" si="13"/>
-        <v>0.12376196447765778</v>
+        <v>0.17827391615908278</v>
       </c>
     </row>
     <row r="122" spans="1:25" x14ac:dyDescent="0.25">
@@ -25895,7 +25897,7 @@
         <v>-0.5905459387483355</v>
       </c>
       <c r="S129" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="130" spans="1:24" x14ac:dyDescent="0.25">
@@ -25970,65 +25972,65 @@
       </c>
       <c r="D131" s="129">
         <f t="shared" ref="C131:O139" si="27">$P131/12</f>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="E131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="F131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="G131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="H131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="I131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="J131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="K131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="L131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="M131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="N131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="O131" s="129">
         <f t="shared" si="27"/>
-        <v>500</v>
+        <v>246.66666666666666</v>
       </c>
       <c r="P131" s="203">
-        <v>6000</v>
+        <v>2960</v>
       </c>
       <c r="Q131" s="128">
         <f t="shared" si="12"/>
-        <v>6000</v>
+        <v>2960</v>
       </c>
       <c r="R131" s="185" t="str">
         <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="S131" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="132" spans="1:24" x14ac:dyDescent="0.25">
@@ -26173,7 +26175,7 @@
         <v>0.72627737226277367</v>
       </c>
       <c r="S133" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="134" spans="1:24" x14ac:dyDescent="0.25">
@@ -26246,7 +26248,7 @@
         <v/>
       </c>
       <c r="S134" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="135" spans="1:24" x14ac:dyDescent="0.25">
@@ -26700,63 +26702,63 @@
       </c>
       <c r="D142" s="130">
         <f t="shared" ref="D142:O142" si="29">SUM(D124:D141)</f>
-        <v>81373.583333333343</v>
+        <v>81120.250000000015</v>
       </c>
       <c r="E142" s="130">
         <f t="shared" si="29"/>
-        <v>2027.3333333333333</v>
+        <v>1774</v>
       </c>
       <c r="F142" s="130">
         <f t="shared" si="29"/>
-        <v>2277.333333333333</v>
+        <v>2024</v>
       </c>
       <c r="G142" s="130">
         <f t="shared" si="29"/>
-        <v>81373.583333333343</v>
+        <v>81120.250000000015</v>
       </c>
       <c r="H142" s="130">
         <f t="shared" si="29"/>
-        <v>2327.3333333333335</v>
+        <v>2074</v>
       </c>
       <c r="I142" s="130">
         <f t="shared" si="29"/>
-        <v>14027.333333333332</v>
+        <v>13773.999999999998</v>
       </c>
       <c r="J142" s="130">
         <f t="shared" si="29"/>
-        <v>81373.583333333343</v>
+        <v>81120.250000000015</v>
       </c>
       <c r="K142" s="130">
         <f t="shared" si="29"/>
-        <v>2027.3333333333333</v>
+        <v>1774</v>
       </c>
       <c r="L142" s="130">
         <f t="shared" si="29"/>
-        <v>2277.333333333333</v>
+        <v>2024</v>
       </c>
       <c r="M142" s="130">
         <f t="shared" si="29"/>
-        <v>81373.583333333343</v>
+        <v>81120.250000000015</v>
       </c>
       <c r="N142" s="130">
         <f t="shared" si="29"/>
-        <v>2027.3333333333333</v>
+        <v>1774</v>
       </c>
       <c r="O142" s="130">
         <f t="shared" si="29"/>
-        <v>2027.3333333333333</v>
+        <v>1774</v>
       </c>
       <c r="P142" s="130">
         <f>SUM(P124:P141)</f>
-        <v>354513</v>
+        <v>351473</v>
       </c>
       <c r="Q142" s="130">
         <f t="shared" si="12"/>
-        <v>26797</v>
+        <v>23757</v>
       </c>
       <c r="R142" s="185">
         <f t="shared" si="13"/>
-        <v>8.1768970694137605E-2</v>
+        <v>7.2492646071598582E-2</v>
       </c>
     </row>
     <row r="143" spans="1:24" x14ac:dyDescent="0.25">
@@ -26890,7 +26892,7 @@
         <v>-0.3</v>
       </c>
       <c r="S145" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V145" s="169"/>
       <c r="W145" s="169"/>
@@ -26959,7 +26961,7 @@
         <v>-0.44350000000000001</v>
       </c>
       <c r="S146" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V146" s="169"/>
       <c r="W146" s="169"/>
@@ -27036,7 +27038,7 @@
         <v>-0.3000000000000001</v>
       </c>
       <c r="S147" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V147" s="169"/>
       <c r="W147" s="169"/>
@@ -27185,7 +27187,7 @@
         <v>-0.3411764705882353</v>
       </c>
       <c r="S149" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="V149" s="164"/>
       <c r="W149" s="164"/>
@@ -27542,63 +27544,63 @@
       </c>
       <c r="D158" s="130">
         <f t="shared" ref="D158:O158" si="38">SUM(D155,D151,D142,D121)</f>
-        <v>139185.21333333335</v>
+        <v>139484.88</v>
       </c>
       <c r="E158" s="130">
         <f t="shared" si="38"/>
-        <v>59700.113333333335</v>
+        <v>59999.78</v>
       </c>
       <c r="F158" s="130">
         <f t="shared" si="38"/>
-        <v>69984.133333333331</v>
+        <v>70283.799999999988</v>
       </c>
       <c r="G158" s="130">
         <f t="shared" si="38"/>
-        <v>150571.98333333334</v>
+        <v>150871.65000000002</v>
       </c>
       <c r="H158" s="130">
         <f t="shared" si="38"/>
-        <v>68390.203333333338</v>
+        <v>68690.87</v>
       </c>
       <c r="I158" s="130">
         <f t="shared" si="38"/>
-        <v>85660.443333333329</v>
+        <v>85960.11</v>
       </c>
       <c r="J158" s="130">
         <f t="shared" si="38"/>
-        <v>137262.61333333334</v>
+        <v>137563.28000000003</v>
       </c>
       <c r="K158" s="130">
         <f t="shared" si="38"/>
-        <v>67984.843333333323</v>
+        <v>68285.509999999995</v>
       </c>
       <c r="L158" s="130">
         <f t="shared" si="38"/>
-        <v>57896.803333333337</v>
+        <v>58197.47</v>
       </c>
       <c r="M158" s="130">
         <f t="shared" si="38"/>
-        <v>137188.37333333335</v>
+        <v>137488.04</v>
       </c>
       <c r="N158" s="130">
         <f t="shared" si="38"/>
-        <v>67880.213333333333</v>
+        <v>68179.88</v>
       </c>
       <c r="O158" s="130">
         <f t="shared" si="38"/>
-        <v>58908.073333333334</v>
+        <v>59207.74</v>
       </c>
       <c r="P158" s="130">
         <f>SUM(P155,P151,P142,P121)</f>
-        <v>1104736.01</v>
+        <v>1118736.01</v>
       </c>
       <c r="Q158" s="130">
         <f t="shared" si="12"/>
-        <v>56234.010000000009</v>
+        <v>70234.010000000009</v>
       </c>
       <c r="R158" s="185">
         <f t="shared" si="13"/>
-        <v>5.3632716008171669E-2</v>
+        <v>6.6985098740870316E-2</v>
       </c>
     </row>
     <row r="159" spans="1:24" x14ac:dyDescent="0.25">
@@ -27666,63 +27668,63 @@
       </c>
       <c r="D161" s="130">
         <f t="shared" si="39"/>
-        <v>-17437.653333333365</v>
+        <v>-17737.320000000022</v>
       </c>
       <c r="E161" s="130">
         <f t="shared" si="39"/>
-        <v>62402.986666666657</v>
+        <v>62103.319999999992</v>
       </c>
       <c r="F161" s="130">
         <f t="shared" si="39"/>
-        <v>52245.166666666672</v>
+        <v>51945.500000000015</v>
       </c>
       <c r="G161" s="130">
         <f t="shared" si="39"/>
-        <v>-28342.683333333334</v>
+        <v>-28642.35000000002</v>
       </c>
       <c r="H161" s="130">
         <f t="shared" si="39"/>
-        <v>54166.776666666672</v>
+        <v>53866.110000000015</v>
       </c>
       <c r="I161" s="130">
         <f t="shared" si="39"/>
-        <v>36896.536666666681</v>
+        <v>36596.87000000001</v>
       </c>
       <c r="J161" s="130">
         <f t="shared" si="39"/>
-        <v>-14705.633333333331</v>
+        <v>-15006.300000000017</v>
       </c>
       <c r="K161" s="130">
         <f t="shared" si="39"/>
-        <v>54602.526666666687</v>
+        <v>54301.860000000015</v>
       </c>
       <c r="L161" s="130">
         <f t="shared" si="39"/>
-        <v>65237.88666666668</v>
+        <v>64937.220000000016</v>
       </c>
       <c r="M161" s="130">
         <f t="shared" si="39"/>
-        <v>-13978.92333333334</v>
+        <v>-14278.589999999997</v>
       </c>
       <c r="N161" s="130">
         <f t="shared" si="39"/>
-        <v>55329.236666666679</v>
+        <v>55029.570000000007</v>
       </c>
       <c r="O161" s="130">
         <f t="shared" si="39"/>
-        <v>64301.376666666678</v>
+        <v>64001.710000000014</v>
       </c>
       <c r="P161" s="130">
         <f t="shared" si="39"/>
-        <v>366589.60000000009</v>
+        <v>352589.60000000009</v>
       </c>
       <c r="Q161" s="130">
         <f t="shared" si="12"/>
-        <v>6369.6000000000931</v>
+        <v>-7630.3999999999069</v>
       </c>
       <c r="R161" s="185">
         <f t="shared" si="13"/>
-        <v>1.7682527344400904E-2</v>
+        <v>-2.1182610626838894E-2</v>
       </c>
     </row>
     <row r="162" spans="1:19" x14ac:dyDescent="0.25">
@@ -27951,21 +27953,21 @@
     <row r="167" spans="1:19" s="173" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A167" s="171"/>
       <c r="B167" s="172"/>
-      <c r="C167" s="222"/>
-      <c r="D167" s="222"/>
-      <c r="E167" s="222"/>
-      <c r="F167" s="222"/>
-      <c r="G167" s="222"/>
-      <c r="H167" s="222"/>
-      <c r="I167" s="222"/>
-      <c r="J167" s="222"/>
-      <c r="K167" s="222"/>
-      <c r="L167" s="222"/>
-      <c r="M167" s="222"/>
-      <c r="N167" s="222"/>
-      <c r="O167" s="222"/>
-      <c r="P167" s="222"/>
-      <c r="Q167" s="222"/>
+      <c r="C167" s="223"/>
+      <c r="D167" s="223"/>
+      <c r="E167" s="223"/>
+      <c r="F167" s="223"/>
+      <c r="G167" s="223"/>
+      <c r="H167" s="223"/>
+      <c r="I167" s="223"/>
+      <c r="J167" s="223"/>
+      <c r="K167" s="223"/>
+      <c r="L167" s="223"/>
+      <c r="M167" s="223"/>
+      <c r="N167" s="223"/>
+      <c r="O167" s="223"/>
+      <c r="P167" s="223"/>
+      <c r="Q167" s="223"/>
       <c r="R167" s="185" t="str">
         <f t="shared" si="40"/>
         <v/>
@@ -28293,20 +28295,21 @@
         <v>0</v>
       </c>
       <c r="E175" s="129">
-        <v>0</v>
+        <f>$P$175/3</f>
+        <v>13333.333333333334</v>
       </c>
       <c r="F175" s="129">
-        <v>0</v>
+        <f t="shared" ref="F175:G175" si="46">$P$175/3</f>
+        <v>13333.333333333334</v>
       </c>
       <c r="G175" s="129">
-        <v>0</v>
+        <f t="shared" si="46"/>
+        <v>13333.333333333334</v>
       </c>
       <c r="H175" s="129">
-        <f>$P$175/2</f>
         <v>0</v>
       </c>
       <c r="I175" s="129">
-        <f>$P$175/2</f>
         <v>0</v>
       </c>
       <c r="J175" s="129">
@@ -28328,18 +28331,18 @@
         <v>0</v>
       </c>
       <c r="P175" s="128">
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q175" s="128">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="R175" s="185" t="str">
         <f t="shared" si="40"/>
         <v/>
       </c>
       <c r="S175" t="s">
-        <v>506</v>
+        <v>580</v>
       </c>
     </row>
     <row r="176" spans="1:19" x14ac:dyDescent="0.25">
@@ -28442,64 +28445,64 @@
         <v>137</v>
       </c>
       <c r="C178" s="130">
-        <f t="shared" ref="C178" si="46">SUM(C175:C177)</f>
+        <f t="shared" ref="C178" si="47">SUM(C175:C177)</f>
         <v>0</v>
       </c>
       <c r="D178" s="130">
-        <f t="shared" ref="D178:O178" si="47">SUM(D175:D177)</f>
+        <f t="shared" ref="D178:O178" si="48">SUM(D175:D177)</f>
         <v>0</v>
       </c>
       <c r="E178" s="130">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="48"/>
+        <v>13333.333333333334</v>
       </c>
       <c r="F178" s="130">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="48"/>
+        <v>13333.333333333334</v>
       </c>
       <c r="G178" s="130">
-        <f t="shared" si="47"/>
-        <v>0</v>
+        <f t="shared" si="48"/>
+        <v>13333.333333333334</v>
       </c>
       <c r="H178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="I178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="J178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="K178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="L178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="M178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="N178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="O178" s="130">
-        <f t="shared" si="47"/>
+        <f t="shared" si="48"/>
         <v>0</v>
       </c>
       <c r="P178" s="130">
         <f>SUM(P175:P177)</f>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="Q178" s="130">
         <f t="shared" si="43"/>
-        <v>0</v>
+        <v>40000</v>
       </c>
       <c r="R178" s="185" t="str">
         <f t="shared" si="40"/>
@@ -28548,60 +28551,60 @@
         <v>68672.2</v>
       </c>
       <c r="E180" s="130">
-        <f t="shared" ref="E180:P180" si="48">SUM(E178,E171,E165)</f>
+        <f t="shared" ref="E180:P180" si="49">SUM(E178,E171,E165)</f>
+        <v>2659.2833333333347</v>
+      </c>
+      <c r="F180" s="130">
+        <f t="shared" si="49"/>
+        <v>15872.283333333336</v>
+      </c>
+      <c r="G180" s="130">
+        <f t="shared" si="49"/>
+        <v>82005.533333333326</v>
+      </c>
+      <c r="H180" s="130">
+        <f t="shared" si="49"/>
         <v>-10674.05</v>
       </c>
-      <c r="F180" s="130">
-        <f t="shared" si="48"/>
+      <c r="I180" s="130">
+        <f t="shared" si="49"/>
         <v>2538.9500000000007</v>
       </c>
-      <c r="G180" s="130">
-        <f t="shared" si="48"/>
+      <c r="J180" s="130">
+        <f t="shared" si="49"/>
         <v>68672.2</v>
       </c>
-      <c r="H180" s="130">
-        <f t="shared" si="48"/>
+      <c r="K180" s="130">
+        <f t="shared" si="49"/>
         <v>-10674.05</v>
       </c>
-      <c r="I180" s="130">
-        <f t="shared" si="48"/>
+      <c r="L180" s="130">
+        <f t="shared" si="49"/>
         <v>2538.9500000000007</v>
       </c>
-      <c r="J180" s="130">
-        <f t="shared" si="48"/>
+      <c r="M180" s="130">
+        <f t="shared" si="49"/>
         <v>68672.2</v>
       </c>
-      <c r="K180" s="130">
-        <f t="shared" si="48"/>
+      <c r="N180" s="130">
+        <f t="shared" si="49"/>
         <v>-10674.05</v>
       </c>
-      <c r="L180" s="130">
-        <f t="shared" si="48"/>
+      <c r="O180" s="130">
+        <f t="shared" si="49"/>
         <v>2538.9500000000007</v>
       </c>
-      <c r="M180" s="130">
-        <f t="shared" si="48"/>
-        <v>68672.2</v>
-      </c>
-      <c r="N180" s="130">
-        <f t="shared" si="48"/>
-        <v>-10674.05</v>
-      </c>
-      <c r="O180" s="130">
-        <f t="shared" si="48"/>
-        <v>2538.9500000000007</v>
-      </c>
       <c r="P180" s="130">
-        <f t="shared" si="48"/>
-        <v>242148.40000000002</v>
+        <f t="shared" si="49"/>
+        <v>282148.40000000002</v>
       </c>
       <c r="Q180" s="130">
         <f t="shared" si="43"/>
-        <v>370237.4</v>
+        <v>410237.4</v>
       </c>
       <c r="R180" s="185">
         <f t="shared" si="40"/>
-        <v>-2.8904699076423426</v>
+        <v>-3.2027527734622021</v>
       </c>
     </row>
     <row r="181" spans="1:31" x14ac:dyDescent="0.25">
@@ -28762,7 +28765,7 @@
       <c r="N184" s="129"/>
       <c r="O184" s="129"/>
       <c r="P184" s="128">
-        <f t="shared" ref="P184" si="49">SUM(D184:O184)</f>
+        <f t="shared" ref="P184" si="50">SUM(D184:O184)</f>
         <v>0</v>
       </c>
       <c r="Q184" s="128" t="str">
@@ -28783,59 +28786,59 @@
         <v>147</v>
       </c>
       <c r="C185" s="130">
-        <f t="shared" ref="C185:P185" si="50">SUM(C183:C184)</f>
+        <f t="shared" ref="C185:P185" si="51">SUM(C183:C184)</f>
         <v>-167996</v>
       </c>
       <c r="D185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14362.450000000004</v>
       </c>
       <c r="E185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14419.300000000003</v>
       </c>
       <c r="F185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14476.380000000005</v>
       </c>
       <c r="G185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14533.68</v>
       </c>
       <c r="H185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14591.210000000006</v>
       </c>
       <c r="I185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14648.970000000001</v>
       </c>
       <c r="J185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14706.950000000004</v>
       </c>
       <c r="K185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14765.170000000006</v>
       </c>
       <c r="L185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14823.61</v>
       </c>
       <c r="M185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14882.29</v>
       </c>
       <c r="N185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-14941.200000000004</v>
       </c>
       <c r="O185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-15000.340000000004</v>
       </c>
       <c r="P185" s="130">
-        <f t="shared" si="50"/>
+        <f t="shared" si="51"/>
         <v>-176151.55000000005</v>
       </c>
       <c r="Q185" s="130">
@@ -28873,7 +28876,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A187" s="1" t="s">
         <v>148</v>
       </c>
@@ -28903,7 +28906,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A188" s="7" t="s">
         <v>436</v>
       </c>
@@ -28933,7 +28936,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A189" s="7" t="s">
         <v>438</v>
       </c>
@@ -28963,7 +28966,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A190" s="7" t="s">
         <v>150</v>
       </c>
@@ -28993,7 +28996,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A191" s="7" t="s">
         <v>151</v>
       </c>
@@ -29023,7 +29026,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="1:31" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:31" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A192" s="7" t="s">
         <v>152</v>
       </c>
@@ -29053,7 +29056,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A193" s="7" t="s">
         <v>443</v>
       </c>
@@ -29083,7 +29086,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A194" s="7" t="s">
         <v>445</v>
       </c>
@@ -29113,7 +29116,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A195" s="7" t="s">
         <v>447</v>
       </c>
@@ -29143,7 +29146,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A196" s="7" t="s">
         <v>449</v>
       </c>
@@ -29173,7 +29176,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A197" s="7" t="s">
         <v>451</v>
       </c>
@@ -29203,7 +29206,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A198" s="7" t="s">
         <v>453</v>
       </c>
@@ -29233,7 +29236,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A199" s="7" t="s">
         <v>455</v>
       </c>
@@ -29263,7 +29266,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A200" s="7" t="s">
         <v>457</v>
       </c>
@@ -29293,7 +29296,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A201" s="7" t="s">
         <v>459</v>
       </c>
@@ -29323,7 +29326,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
         <v>461</v>
       </c>
@@ -29353,7 +29356,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A203" s="7" t="s">
         <v>463</v>
       </c>
@@ -29383,7 +29386,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="1:18" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:18" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A204" s="7" t="s">
         <v>465</v>
       </c>
@@ -29413,7 +29416,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="1:18" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:18" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A205" s="7" t="s">
         <v>467</v>
       </c>
@@ -29443,7 +29446,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="1:18" s="121" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:18" s="121" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A206" s="6" t="s">
         <v>153</v>
       </c>
@@ -29451,59 +29454,59 @@
         <v>154</v>
       </c>
       <c r="C206" s="130">
-        <f t="shared" ref="C206:P206" si="51">SUM(C188:C205)</f>
+        <f t="shared" ref="C206:P206" si="52">SUM(C188:C205)</f>
         <v>0</v>
       </c>
       <c r="D206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="E206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="F206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="G206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="H206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="I206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="J206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="K206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="L206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="M206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="N206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="O206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="P206" s="130">
-        <f t="shared" si="51"/>
+        <f t="shared" si="52"/>
         <v>0</v>
       </c>
       <c r="Q206" s="130">
@@ -29541,7 +29544,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A208" s="1" t="s">
         <v>155</v>
       </c>
@@ -29571,12 +29574,12 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A209" s="188" t="s">
+        <v>534</v>
+      </c>
+      <c r="B209" s="5" t="s">
         <v>535</v>
-      </c>
-      <c r="B209" s="5" t="s">
-        <v>536</v>
       </c>
       <c r="C209" s="128">
         <v>-34074</v>
@@ -29630,7 +29633,7 @@
         <v>-2839.5</v>
       </c>
       <c r="P209" s="128">
-        <f t="shared" ref="P209:P219" si="52">SUM(D209:O209)</f>
+        <f t="shared" ref="P209:P219" si="53">SUM(D209:O209)</f>
         <v>-34074</v>
       </c>
       <c r="Q209" s="128">
@@ -29652,12 +29655,12 @@
       <c r="AA209" s="140"/>
       <c r="AB209" s="140"/>
     </row>
-    <row r="210" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A210" s="188" t="s">
+        <v>536</v>
+      </c>
+      <c r="B210" s="5" t="s">
         <v>537</v>
-      </c>
-      <c r="B210" s="5" t="s">
-        <v>538</v>
       </c>
       <c r="C210" s="128">
         <v>-17028</v>
@@ -29711,7 +29714,7 @@
         <v>-1419</v>
       </c>
       <c r="P210" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-17028</v>
       </c>
       <c r="Q210" s="128">
@@ -29733,12 +29736,12 @@
       <c r="AA210" s="140"/>
       <c r="AB210" s="140"/>
     </row>
-    <row r="211" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A211" s="188" t="s">
+        <v>538</v>
+      </c>
+      <c r="B211" s="5" t="s">
         <v>539</v>
-      </c>
-      <c r="B211" s="5" t="s">
-        <v>540</v>
       </c>
       <c r="C211" s="128">
         <v>-51192</v>
@@ -29792,7 +29795,7 @@
         <v>-4266</v>
       </c>
       <c r="P211" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-51192</v>
       </c>
       <c r="Q211" s="128">
@@ -29814,12 +29817,12 @@
       <c r="AA211" s="140"/>
       <c r="AB211" s="140"/>
     </row>
-    <row r="212" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A212" s="188" t="s">
         <v>157</v>
       </c>
       <c r="B212" s="5" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C212" s="128">
         <v>-36000</v>
@@ -29873,7 +29876,7 @@
         <v>-3000</v>
       </c>
       <c r="P212" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-36000</v>
       </c>
       <c r="Q212" s="128">
@@ -29895,12 +29898,12 @@
       <c r="AA212" s="140"/>
       <c r="AB212" s="140"/>
     </row>
-    <row r="213" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A213" s="188" t="s">
+        <v>541</v>
+      </c>
+      <c r="B213" s="5" t="s">
         <v>542</v>
-      </c>
-      <c r="B213" s="5" t="s">
-        <v>543</v>
       </c>
       <c r="C213" s="128">
         <v>-51192</v>
@@ -29954,7 +29957,7 @@
         <v>-4266</v>
       </c>
       <c r="P213" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-51192</v>
       </c>
       <c r="Q213" s="128">
@@ -29976,12 +29979,12 @@
       <c r="AA213" s="140"/>
       <c r="AB213" s="140"/>
     </row>
-    <row r="214" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A214" s="188" t="s">
         <v>435</v>
       </c>
       <c r="B214" s="5" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C214" s="128">
         <v>-17028</v>
@@ -30035,7 +30038,7 @@
         <v>-1419</v>
       </c>
       <c r="P214" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-17028</v>
       </c>
       <c r="Q214" s="128">
@@ -30057,12 +30060,12 @@
       <c r="AA214" s="140"/>
       <c r="AB214" s="140"/>
     </row>
-    <row r="215" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A215" s="188" t="s">
+        <v>544</v>
+      </c>
+      <c r="B215" s="5" t="s">
         <v>545</v>
-      </c>
-      <c r="B215" s="5" t="s">
-        <v>546</v>
       </c>
       <c r="C215" s="128">
         <v>-17028</v>
@@ -30116,7 +30119,7 @@
         <v>-1419</v>
       </c>
       <c r="P215" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-17028</v>
       </c>
       <c r="Q215" s="128">
@@ -30138,12 +30141,12 @@
       <c r="AA215" s="140"/>
       <c r="AB215" s="140"/>
     </row>
-    <row r="216" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A216" s="188" t="s">
+        <v>546</v>
+      </c>
+      <c r="B216" s="5" t="s">
         <v>547</v>
-      </c>
-      <c r="B216" s="5" t="s">
-        <v>548</v>
       </c>
       <c r="C216" s="128">
         <v>-34074</v>
@@ -30197,7 +30200,7 @@
         <v>-2839.5</v>
       </c>
       <c r="P216" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-34074</v>
       </c>
       <c r="Q216" s="128">
@@ -30219,12 +30222,12 @@
       <c r="AA216" s="140"/>
       <c r="AB216" s="140"/>
     </row>
-    <row r="217" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A217" s="188" t="s">
+        <v>548</v>
+      </c>
+      <c r="B217" s="5" t="s">
         <v>549</v>
-      </c>
-      <c r="B217" s="5" t="s">
-        <v>550</v>
       </c>
       <c r="C217" s="128">
         <v>-25596</v>
@@ -30278,7 +30281,7 @@
         <v>-2133</v>
       </c>
       <c r="P217" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-25596</v>
       </c>
       <c r="Q217" s="128">
@@ -30300,12 +30303,12 @@
       <c r="AA217" s="140"/>
       <c r="AB217" s="140"/>
     </row>
-    <row r="218" spans="1:28" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:28" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A218" s="188" t="s">
+        <v>550</v>
+      </c>
+      <c r="B218" s="5" t="s">
         <v>551</v>
-      </c>
-      <c r="B218" s="5" t="s">
-        <v>552</v>
       </c>
       <c r="C218" s="128">
         <v>-25596</v>
@@ -30359,7 +30362,7 @@
         <v>-2133</v>
       </c>
       <c r="P218" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-25596</v>
       </c>
       <c r="Q218" s="128">
@@ -30381,12 +30384,12 @@
       <c r="AA218" s="140"/>
       <c r="AB218" s="140"/>
     </row>
-    <row r="219" spans="1:28" ht="15.75" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:28" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A219" s="188" t="s">
+        <v>552</v>
+      </c>
+      <c r="B219" s="5" t="s">
         <v>553</v>
-      </c>
-      <c r="B219" s="5" t="s">
-        <v>554</v>
       </c>
       <c r="C219" s="128">
         <v>-51192</v>
@@ -30440,7 +30443,7 @@
         <v>-4266</v>
       </c>
       <c r="P219" s="128">
-        <f t="shared" si="52"/>
+        <f t="shared" si="53"/>
         <v>-51192</v>
       </c>
       <c r="Q219" s="128">
@@ -30462,7 +30465,7 @@
       <c r="AA219" s="140"/>
       <c r="AB219" s="140"/>
     </row>
-    <row r="220" spans="1:28" s="121" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:28" s="121" customFormat="1" collapsed="1" x14ac:dyDescent="0.25">
       <c r="A220" s="6" t="s">
         <v>158</v>
       </c>
@@ -30470,59 +30473,59 @@
         <v>159</v>
       </c>
       <c r="C220" s="130">
-        <f t="shared" ref="C220:P220" si="53">SUM(C209:C219)</f>
+        <f t="shared" ref="C220:P220" si="54">SUM(C209:C219)</f>
         <v>-360000</v>
       </c>
       <c r="D220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="E220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="F220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="G220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="H220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="I220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="J220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="K220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="L220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="M220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="N220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="O220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-30000</v>
       </c>
       <c r="P220" s="130">
-        <f t="shared" si="53"/>
+        <f t="shared" si="54"/>
         <v>-360000</v>
       </c>
       <c r="Q220" s="130">
@@ -30530,7 +30533,7 @@
         <v>0</v>
       </c>
       <c r="R220" s="185">
-        <f t="shared" ref="R220:R225" si="54">IF(C220&lt;&gt;0,Q220/C220,"")</f>
+        <f t="shared" ref="R220:R225" si="55">IF(C220&lt;&gt;0,Q220/C220,"")</f>
         <v>0</v>
       </c>
     </row>
@@ -30555,7 +30558,7 @@
         <v/>
       </c>
       <c r="R221" s="185" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
     </row>
@@ -30581,7 +30584,7 @@
         <v/>
       </c>
       <c r="R222" s="185" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
     </row>
@@ -30591,68 +30594,68 @@
         <v>160</v>
       </c>
       <c r="C223" s="130">
-        <f t="shared" ref="C223:P223" si="55">C180+C185+C206+C220</f>
+        <f t="shared" ref="C223:P223" si="56">C180+C185+C206+C220</f>
         <v>-656085</v>
       </c>
       <c r="D223" s="130">
+        <f t="shared" si="56"/>
+        <v>24309.749999999993</v>
+      </c>
+      <c r="E223" s="130">
+        <f t="shared" si="56"/>
+        <v>-41760.01666666667</v>
+      </c>
+      <c r="F223" s="130">
+        <f t="shared" si="56"/>
+        <v>-28604.096666666668</v>
+      </c>
+      <c r="G223" s="130">
+        <f t="shared" si="56"/>
+        <v>37471.853333333333</v>
+      </c>
+      <c r="H223" s="130">
+        <f t="shared" si="56"/>
+        <v>-55265.260000000009</v>
+      </c>
+      <c r="I223" s="130">
+        <f t="shared" si="56"/>
+        <v>-42110.020000000004</v>
+      </c>
+      <c r="J223" s="130">
+        <f t="shared" si="56"/>
+        <v>23965.249999999993</v>
+      </c>
+      <c r="K223" s="130">
+        <f t="shared" si="56"/>
+        <v>-55439.22</v>
+      </c>
+      <c r="L223" s="130">
+        <f t="shared" si="56"/>
+        <v>-42284.66</v>
+      </c>
+      <c r="M223" s="130">
+        <f t="shared" si="56"/>
+        <v>23789.909999999996</v>
+      </c>
+      <c r="N223" s="130">
+        <f t="shared" si="56"/>
+        <v>-55615.25</v>
+      </c>
+      <c r="O223" s="130">
+        <f t="shared" si="56"/>
+        <v>-42461.39</v>
+      </c>
+      <c r="P223" s="130">
+        <f t="shared" si="56"/>
+        <v>-254003.15000000002</v>
+      </c>
+      <c r="Q223" s="130">
+        <f t="shared" ref="Q223:Q225" si="57">IF(C223&lt;&gt;"",P223-C223,"")</f>
+        <v>402081.85</v>
+      </c>
+      <c r="R223" s="185">
         <f t="shared" si="55"/>
-        <v>24309.749999999993</v>
-      </c>
-      <c r="E223" s="130">
-        <f t="shared" si="55"/>
-        <v>-55093.350000000006</v>
-      </c>
-      <c r="F223" s="130">
-        <f t="shared" si="55"/>
-        <v>-41937.430000000008</v>
-      </c>
-      <c r="G223" s="130">
-        <f t="shared" si="55"/>
-        <v>24138.519999999997</v>
-      </c>
-      <c r="H223" s="130">
-        <f t="shared" si="55"/>
-        <v>-55265.260000000009</v>
-      </c>
-      <c r="I223" s="130">
-        <f t="shared" si="55"/>
-        <v>-42110.020000000004</v>
-      </c>
-      <c r="J223" s="130">
-        <f t="shared" si="55"/>
-        <v>23965.249999999993</v>
-      </c>
-      <c r="K223" s="130">
-        <f t="shared" si="55"/>
-        <v>-55439.22</v>
-      </c>
-      <c r="L223" s="130">
-        <f t="shared" si="55"/>
-        <v>-42284.66</v>
-      </c>
-      <c r="M223" s="130">
-        <f t="shared" si="55"/>
-        <v>23789.909999999996</v>
-      </c>
-      <c r="N223" s="130">
-        <f t="shared" si="55"/>
-        <v>-55615.25</v>
-      </c>
-      <c r="O223" s="130">
-        <f t="shared" si="55"/>
-        <v>-42461.39</v>
-      </c>
-      <c r="P223" s="130">
-        <f t="shared" si="55"/>
-        <v>-294003.15000000002</v>
-      </c>
-      <c r="Q223" s="130">
-        <f t="shared" ref="Q223:Q225" si="56">IF(C223&lt;&gt;"",P223-C223,"")</f>
-        <v>362081.85</v>
-      </c>
-      <c r="R223" s="185">
-        <f t="shared" si="54"/>
-        <v>-0.55188253046480251</v>
+        <v>-0.61285024044140624</v>
       </c>
     </row>
     <row r="224" spans="1:28" s="121" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30673,11 +30676,11 @@
       <c r="O224" s="137"/>
       <c r="P224" s="137"/>
       <c r="Q224" s="137" t="str">
-        <f t="shared" si="56"/>
+        <f t="shared" si="57"/>
         <v/>
       </c>
       <c r="R224" s="185" t="str">
-        <f t="shared" si="54"/>
+        <f t="shared" si="55"/>
         <v/>
       </c>
     </row>
@@ -30687,68 +30690,68 @@
         <v>161</v>
       </c>
       <c r="C225" s="130">
-        <f t="shared" ref="C225:P225" si="57">SUM(C223,C161)</f>
+        <f t="shared" ref="C225:P225" si="58">SUM(C223,C161)</f>
         <v>-295865</v>
       </c>
       <c r="D225" s="130">
+        <f t="shared" si="58"/>
+        <v>6572.4299999999712</v>
+      </c>
+      <c r="E225" s="130">
+        <f t="shared" si="58"/>
+        <v>20343.303333333322</v>
+      </c>
+      <c r="F225" s="130">
+        <f t="shared" si="58"/>
+        <v>23341.403333333346</v>
+      </c>
+      <c r="G225" s="130">
+        <f t="shared" si="58"/>
+        <v>8829.5033333333122</v>
+      </c>
+      <c r="H225" s="130">
+        <f t="shared" si="58"/>
+        <v>-1399.1499999999942</v>
+      </c>
+      <c r="I225" s="130">
+        <f t="shared" si="58"/>
+        <v>-5513.1499999999942</v>
+      </c>
+      <c r="J225" s="130">
+        <f t="shared" si="58"/>
+        <v>8958.9499999999753</v>
+      </c>
+      <c r="K225" s="130">
+        <f t="shared" si="58"/>
+        <v>-1137.359999999986</v>
+      </c>
+      <c r="L225" s="130">
+        <f t="shared" si="58"/>
+        <v>22652.560000000012</v>
+      </c>
+      <c r="M225" s="130">
+        <f t="shared" si="58"/>
+        <v>9511.32</v>
+      </c>
+      <c r="N225" s="130">
+        <f t="shared" si="58"/>
+        <v>-585.67999999999302</v>
+      </c>
+      <c r="O225" s="130">
+        <f t="shared" si="58"/>
+        <v>21540.320000000014</v>
+      </c>
+      <c r="P225" s="130">
+        <f t="shared" si="58"/>
+        <v>98586.45000000007</v>
+      </c>
+      <c r="Q225" s="130">
         <f t="shared" si="57"/>
-        <v>6872.0966666666282</v>
-      </c>
-      <c r="E225" s="130">
-        <f t="shared" si="57"/>
-        <v>7309.6366666666509</v>
-      </c>
-      <c r="F225" s="130">
-        <f t="shared" si="57"/>
-        <v>10307.736666666664</v>
-      </c>
-      <c r="G225" s="130">
-        <f t="shared" si="57"/>
-        <v>-4204.1633333333375</v>
-      </c>
-      <c r="H225" s="130">
-        <f t="shared" si="57"/>
-        <v>-1098.4833333333372</v>
-      </c>
-      <c r="I225" s="130">
-        <f t="shared" si="57"/>
-        <v>-5213.4833333333227</v>
-      </c>
-      <c r="J225" s="130">
-        <f t="shared" si="57"/>
-        <v>9259.6166666666613</v>
-      </c>
-      <c r="K225" s="130">
-        <f t="shared" si="57"/>
-        <v>-836.69333333331451</v>
-      </c>
-      <c r="L225" s="130">
-        <f t="shared" si="57"/>
-        <v>22953.226666666676</v>
-      </c>
-      <c r="M225" s="130">
-        <f t="shared" si="57"/>
-        <v>9810.9866666666567</v>
-      </c>
-      <c r="N225" s="130">
-        <f t="shared" si="57"/>
-        <v>-286.0133333333215</v>
-      </c>
-      <c r="O225" s="130">
-        <f t="shared" si="57"/>
-        <v>21839.986666666679</v>
-      </c>
-      <c r="P225" s="130">
-        <f t="shared" si="57"/>
-        <v>72586.45000000007</v>
-      </c>
-      <c r="Q225" s="130">
-        <f t="shared" si="56"/>
-        <v>368451.45000000007</v>
+        <v>394451.45000000007</v>
       </c>
       <c r="R225" s="185">
-        <f t="shared" si="54"/>
-        <v>-1.2453363865276394</v>
+        <f t="shared" si="55"/>
+        <v>-1.3332143038209996</v>
       </c>
     </row>
     <row r="226" spans="1:18" s="121" customFormat="1" x14ac:dyDescent="0.25">
@@ -30780,47 +30783,47 @@
       <c r="D227" s="139"/>
       <c r="E227" s="139">
         <f>D228</f>
-        <v>6872.0966666666282</v>
+        <v>6572.4299999999712</v>
       </c>
       <c r="F227" s="139">
-        <f t="shared" ref="F227:O227" si="58">E228</f>
-        <v>14181.733333333279</v>
+        <f t="shared" ref="F227:O227" si="59">E228</f>
+        <v>26915.733333333294</v>
       </c>
       <c r="G227" s="139">
-        <f t="shared" si="58"/>
-        <v>24489.469999999943</v>
+        <f t="shared" si="59"/>
+        <v>50257.136666666644</v>
       </c>
       <c r="H227" s="139">
-        <f t="shared" si="58"/>
-        <v>20285.306666666605</v>
+        <f t="shared" si="59"/>
+        <v>59086.639999999956</v>
       </c>
       <c r="I227" s="139">
-        <f t="shared" si="58"/>
-        <v>19186.823333333268</v>
+        <f t="shared" si="59"/>
+        <v>57687.489999999962</v>
       </c>
       <c r="J227" s="139">
-        <f t="shared" si="58"/>
-        <v>13973.339999999946</v>
+        <f t="shared" si="59"/>
+        <v>52174.339999999967</v>
       </c>
       <c r="K227" s="139">
-        <f t="shared" si="58"/>
-        <v>23232.956666666607</v>
+        <f t="shared" si="59"/>
+        <v>61133.289999999943</v>
       </c>
       <c r="L227" s="139">
-        <f t="shared" si="58"/>
-        <v>22396.263333333292</v>
+        <f t="shared" si="59"/>
+        <v>59995.929999999957</v>
       </c>
       <c r="M227" s="139">
-        <f t="shared" si="58"/>
-        <v>45349.489999999969</v>
+        <f t="shared" si="59"/>
+        <v>82648.489999999962</v>
       </c>
       <c r="N227" s="139">
-        <f t="shared" si="58"/>
-        <v>55160.476666666626</v>
+        <f t="shared" si="59"/>
+        <v>92159.809999999969</v>
       </c>
       <c r="O227" s="139">
-        <f t="shared" si="58"/>
-        <v>54874.463333333304</v>
+        <f t="shared" si="59"/>
+        <v>91574.129999999976</v>
       </c>
       <c r="P227" s="138"/>
       <c r="Q227" s="138"/>
@@ -30834,51 +30837,51 @@
       <c r="C228" s="139"/>
       <c r="D228" s="139">
         <f>D227+D225</f>
-        <v>6872.0966666666282</v>
+        <v>6572.4299999999712</v>
       </c>
       <c r="E228" s="139">
         <f>E227+E225</f>
-        <v>14181.733333333279</v>
+        <v>26915.733333333294</v>
       </c>
       <c r="F228" s="139">
-        <f t="shared" ref="F228:O228" si="59">F227+F225</f>
-        <v>24489.469999999943</v>
+        <f t="shared" ref="F228:O228" si="60">F227+F225</f>
+        <v>50257.136666666644</v>
       </c>
       <c r="G228" s="139">
-        <f t="shared" si="59"/>
-        <v>20285.306666666605</v>
+        <f t="shared" si="60"/>
+        <v>59086.639999999956</v>
       </c>
       <c r="H228" s="139">
-        <f t="shared" si="59"/>
-        <v>19186.823333333268</v>
+        <f t="shared" si="60"/>
+        <v>57687.489999999962</v>
       </c>
       <c r="I228" s="139">
-        <f t="shared" si="59"/>
-        <v>13973.339999999946</v>
+        <f t="shared" si="60"/>
+        <v>52174.339999999967</v>
       </c>
       <c r="J228" s="139">
-        <f t="shared" si="59"/>
-        <v>23232.956666666607</v>
+        <f t="shared" si="60"/>
+        <v>61133.289999999943</v>
       </c>
       <c r="K228" s="139">
-        <f t="shared" si="59"/>
-        <v>22396.263333333292</v>
+        <f t="shared" si="60"/>
+        <v>59995.929999999957</v>
       </c>
       <c r="L228" s="139">
-        <f t="shared" si="59"/>
-        <v>45349.489999999969</v>
+        <f t="shared" si="60"/>
+        <v>82648.489999999962</v>
       </c>
       <c r="M228" s="139">
-        <f t="shared" si="59"/>
-        <v>55160.476666666626</v>
+        <f t="shared" si="60"/>
+        <v>92159.809999999969</v>
       </c>
       <c r="N228" s="139">
-        <f t="shared" si="59"/>
-        <v>54874.463333333304</v>
+        <f t="shared" si="60"/>
+        <v>91574.129999999976</v>
       </c>
       <c r="O228" s="139">
-        <f t="shared" si="59"/>
-        <v>76714.449999999983</v>
+        <f t="shared" si="60"/>
+        <v>113114.44999999998</v>
       </c>
       <c r="P228" s="139"/>
       <c r="Q228" s="139"/>
@@ -30967,7 +30970,7 @@
     <row r="233" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A233" s="1"/>
       <c r="B233" s="5" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="C233" s="129"/>
       <c r="D233" s="128">
@@ -30978,43 +30981,43 @@
         <v>-583.49</v>
       </c>
       <c r="F233" s="128">
-        <f t="shared" ref="F233:O233" si="60">E233</f>
+        <f t="shared" ref="F233:O233" si="61">E233</f>
         <v>-583.49</v>
       </c>
       <c r="G233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="H233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="I233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="J233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="K233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="L233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="M233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="N233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="O233" s="128">
-        <f t="shared" si="60"/>
+        <f t="shared" si="61"/>
         <v>-583.49</v>
       </c>
       <c r="P233" s="128">
@@ -31064,7 +31067,7 @@
       <c r="N235" s="128"/>
       <c r="O235" s="128"/>
       <c r="P235" s="128">
-        <f t="shared" ref="P235" si="61">SUM(D235:O235)</f>
+        <f t="shared" ref="P235" si="62">SUM(D235:O235)</f>
         <v>0</v>
       </c>
       <c r="Q235" s="129"/>
@@ -31099,55 +31102,55 @@
       </c>
       <c r="C237"/>
       <c r="D237" s="130">
-        <f t="shared" ref="D237:P237" si="62">SUM(D233:D236)</f>
+        <f t="shared" ref="D237:P237" si="63">SUM(D233:D236)</f>
         <v>-583.49</v>
       </c>
       <c r="E237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="F237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="G237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="H237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="I237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="J237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="K237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="L237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="M237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="N237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="O237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-583.49</v>
       </c>
       <c r="P237" s="130">
-        <f t="shared" si="62"/>
+        <f t="shared" si="63"/>
         <v>-7001.8799999999983</v>
       </c>
       <c r="Q237"/>
@@ -31194,63 +31197,63 @@
     </row>
     <row r="240" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A240" s="122" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>494</v>
       </c>
       <c r="C240" s="129"/>
       <c r="D240" s="134">
-        <f t="shared" ref="D240:P240" si="63">D225+D237</f>
-        <v>6288.6066666666284</v>
+        <f t="shared" ref="D240:P240" si="64">D225+D237</f>
+        <v>5988.9399999999714</v>
       </c>
       <c r="E240" s="134">
-        <f t="shared" si="63"/>
-        <v>6726.1466666666511</v>
+        <f t="shared" si="64"/>
+        <v>19759.813333333321</v>
       </c>
       <c r="F240" s="134">
-        <f t="shared" si="63"/>
-        <v>9724.2466666666642</v>
+        <f t="shared" si="64"/>
+        <v>22757.913333333345</v>
       </c>
       <c r="G240" s="134">
-        <f t="shared" si="63"/>
-        <v>-4787.6533333333373</v>
+        <f t="shared" si="64"/>
+        <v>8246.0133333333124</v>
       </c>
       <c r="H240" s="134">
-        <f t="shared" si="63"/>
-        <v>-1681.9733333333372</v>
+        <f t="shared" si="64"/>
+        <v>-1982.6399999999942</v>
       </c>
       <c r="I240" s="134">
-        <f t="shared" si="63"/>
-        <v>-5796.9733333333224</v>
+        <f t="shared" si="64"/>
+        <v>-6096.639999999994</v>
       </c>
       <c r="J240" s="134">
-        <f t="shared" si="63"/>
-        <v>8676.1266666666615</v>
+        <f t="shared" si="64"/>
+        <v>8375.4599999999755</v>
       </c>
       <c r="K240" s="134">
-        <f t="shared" si="63"/>
-        <v>-1420.1833333333145</v>
+        <f t="shared" si="64"/>
+        <v>-1720.849999999986</v>
       </c>
       <c r="L240" s="134">
-        <f t="shared" si="63"/>
-        <v>22369.736666666675</v>
+        <f t="shared" si="64"/>
+        <v>22069.070000000011</v>
       </c>
       <c r="M240" s="134">
-        <f t="shared" si="63"/>
-        <v>9227.4966666666569</v>
+        <f t="shared" si="64"/>
+        <v>8927.83</v>
       </c>
       <c r="N240" s="134">
-        <f t="shared" si="63"/>
-        <v>-869.50333333332151</v>
+        <f t="shared" si="64"/>
+        <v>-1169.169999999993</v>
       </c>
       <c r="O240" s="134">
-        <f t="shared" si="63"/>
-        <v>21256.496666666677</v>
+        <f t="shared" si="64"/>
+        <v>20956.830000000013</v>
       </c>
       <c r="P240" s="134">
-        <f t="shared" si="63"/>
-        <v>65584.570000000065</v>
+        <f t="shared" si="64"/>
+        <v>91584.570000000065</v>
       </c>
       <c r="Q240" s="129"/>
       <c r="R240" s="184"/>
@@ -31440,10 +31443,10 @@
     </row>
     <row r="5" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="189" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B5" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C5" s="190"/>
       <c r="D5" s="191">
@@ -31507,10 +31510,10 @@
     </row>
     <row r="6" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B6" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C6" s="190"/>
       <c r="D6" s="191">
@@ -31573,10 +31576,10 @@
     </row>
     <row r="7" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B7" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C7" s="190"/>
       <c r="D7" s="191">
@@ -31640,10 +31643,10 @@
     </row>
     <row r="8" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B8" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C8" s="190"/>
       <c r="D8" s="191">
@@ -31707,10 +31710,10 @@
     </row>
     <row r="9" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B9" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C9" s="190"/>
       <c r="D9" s="191">
@@ -31774,10 +31777,10 @@
     </row>
     <row r="10" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B10" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C10" s="190"/>
       <c r="D10" s="190">
@@ -31841,10 +31844,10 @@
     </row>
     <row r="11" spans="1:21" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B11" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C11" s="192"/>
       <c r="D11" s="190">
@@ -31911,10 +31914,10 @@
     </row>
     <row r="12" spans="1:21" s="193" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="193" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B12" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C12" s="194"/>
       <c r="D12" s="194">
@@ -31977,10 +31980,10 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B13" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D13" s="102">
         <v>13.999979999999999</v>
@@ -32045,10 +32048,10 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B14" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D14" s="102">
         <v>16.163636363636364</v>
@@ -32109,10 +32112,10 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B15" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D15" s="102">
         <v>0</v>
@@ -32173,10 +32176,10 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B16" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D16" s="102">
         <v>9.5276923076923072</v>
@@ -32238,10 +32241,10 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B17" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D17" s="102">
         <v>27.867999999999999</v>
@@ -32303,10 +32306,10 @@
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B18" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D18" s="102">
         <v>22</v>
@@ -32371,10 +32374,10 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" s="125" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B19" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="D19" s="102">
         <v>13.383200000000002</v>
@@ -32435,10 +32438,10 @@
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" s="31" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B20" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E20" s="103">
         <v>3111.9700000000003</v>
@@ -32496,10 +32499,10 @@
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" s="31" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B21" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E21" s="103">
         <v>5611.67</v>
@@ -32558,10 +32561,10 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" s="31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B22" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E22" s="103">
         <v>4206.76</v>
@@ -32619,10 +32622,10 @@
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" s="31" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B23" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E23" s="103">
         <v>14251.76</v>
@@ -32680,10 +32683,10 @@
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" s="31" t="s">
+        <v>530</v>
+      </c>
+      <c r="B24" s="197" t="s">
         <v>531</v>
-      </c>
-      <c r="B24" s="197" t="s">
-        <v>532</v>
       </c>
       <c r="E24" s="103">
         <v>10118.27</v>
@@ -32742,7 +32745,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" s="125" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="Q25" s="103">
         <f t="shared" si="2"/>
@@ -32754,7 +32757,7 @@
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" s="125" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="Q26" s="103">
         <f t="shared" si="2"/>
@@ -32953,10 +32956,10 @@
     </row>
     <row r="6" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C6" s="190">
         <v>2850</v>
@@ -33019,10 +33022,10 @@
     </row>
     <row r="7" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="54" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C7" s="190">
         <f>12835+1958+2403</f>
@@ -33086,10 +33089,10 @@
     </row>
     <row r="8" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="54" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C8" s="190">
         <v>1240</v>
@@ -33152,10 +33155,10 @@
     </row>
     <row r="9" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="54" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C9" s="190">
         <v>976</v>
@@ -33218,10 +33221,10 @@
     </row>
     <row r="10" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C10" s="190">
         <v>1216</v>
@@ -33284,10 +33287,10 @@
     </row>
     <row r="11" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="54" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C11" s="190">
         <v>24000</v>
@@ -33353,10 +33356,10 @@
     </row>
     <row r="12" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="54" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B12" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C12" s="192">
         <v>2000</v>
@@ -33422,10 +33425,10 @@
     </row>
     <row r="13" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="193" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B13" s="59" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C13" s="194">
         <v>1980</v>
@@ -33491,10 +33494,10 @@
     </row>
     <row r="14" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="54" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B14" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C14" s="190">
         <v>2000</v>
@@ -33557,10 +33560,10 @@
     </row>
     <row r="15" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="54" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B15" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C15" s="190">
         <v>1980</v>
@@ -33623,10 +33626,10 @@
     </row>
     <row r="16" spans="1:20" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="54" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B16" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C16" s="190">
         <v>2000</v>
@@ -33689,10 +33692,10 @@
     </row>
     <row r="17" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="54" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B17" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C17" s="190">
         <v>7800</v>
@@ -33755,10 +33758,10 @@
     </row>
     <row r="18" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="54" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B18" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C18" s="190">
         <v>3000</v>
@@ -33821,10 +33824,10 @@
     </row>
     <row r="19" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="54" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B19" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C19" s="190">
         <v>8700</v>
@@ -33887,10 +33890,10 @@
     </row>
     <row r="20" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="189" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B20" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C20" s="190">
         <v>3000</v>
@@ -33953,10 +33956,10 @@
     </row>
     <row r="21" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="189" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B21" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C21" s="190"/>
       <c r="D21" s="190"/>
@@ -34015,10 +34018,10 @@
     </row>
     <row r="22" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="189" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B22" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C22" s="190"/>
       <c r="D22" s="190"/>
@@ -34077,10 +34080,10 @@
     </row>
     <row r="23" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="189" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="B23" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C23" s="190"/>
       <c r="D23" s="190"/>
@@ -34136,10 +34139,10 @@
     </row>
     <row r="24" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="189" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="B24" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C24" s="190"/>
       <c r="D24" s="190"/>
@@ -34195,10 +34198,10 @@
     </row>
     <row r="25" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="189" t="s">
+        <v>530</v>
+      </c>
+      <c r="B25" s="197" t="s">
         <v>531</v>
-      </c>
-      <c r="B25" s="197" t="s">
-        <v>532</v>
       </c>
       <c r="C25" s="190"/>
       <c r="D25" s="190"/>
@@ -34254,10 +34257,10 @@
     </row>
     <row r="26" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="189" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B26" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C26" s="190"/>
       <c r="D26" s="190"/>
@@ -34311,10 +34314,10 @@
     </row>
     <row r="27" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="189" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B27" s="197" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C27" s="190"/>
       <c r="D27" s="190"/>
@@ -34556,7 +34559,7 @@
     </row>
     <row r="6" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>404</v>
@@ -34611,7 +34614,7 @@
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>404</v>
@@ -34666,7 +34669,7 @@
     </row>
     <row r="8" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>404</v>
@@ -34721,7 +34724,7 @@
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>404</v>
@@ -34775,7 +34778,7 @@
     </row>
     <row r="10" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>404</v>
@@ -34830,7 +34833,7 @@
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>404</v>
@@ -34887,7 +34890,7 @@
     </row>
     <row r="12" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>404</v>
@@ -34945,7 +34948,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="112" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B13" s="113" t="s">
         <v>404</v>
@@ -35002,7 +35005,7 @@
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>404</v>
@@ -35056,7 +35059,7 @@
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>404</v>
@@ -35110,7 +35113,7 @@
     </row>
     <row r="16" spans="1:20" s="117" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>404</v>
@@ -35165,7 +35168,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>404</v>
@@ -35219,7 +35222,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>404</v>
@@ -35273,7 +35276,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>404</v>
@@ -35327,7 +35330,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="125" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>404</v>
@@ -35381,7 +35384,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="125" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="E21" s="103">
         <v>0</v>
@@ -35422,7 +35425,7 @@
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="125" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="E22" s="103">
         <v>0</v>
@@ -35463,7 +35466,7 @@
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="125" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="E23" s="103">
         <v>0</v>
@@ -35504,7 +35507,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="125" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="E24" s="103">
         <v>0</v>
@@ -35545,7 +35548,7 @@
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="125" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="E25" s="103">
         <v>0</v>
@@ -35586,7 +35589,7 @@
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="125" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="E26" s="103">
         <v>0</v>
@@ -35627,7 +35630,7 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="125" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="E27" s="103">
         <v>0</v>
@@ -35832,7 +35835,7 @@
     </row>
     <row r="6" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="31" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="B6" s="32" t="s">
         <v>404</v>
@@ -35886,7 +35889,7 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B7" s="25" t="s">
         <v>404</v>
@@ -35941,7 +35944,7 @@
     </row>
     <row r="8" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="31" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>404</v>
@@ -35995,7 +35998,7 @@
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>404</v>
@@ -36049,7 +36052,7 @@
     </row>
     <row r="10" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="31" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B10" s="32" t="s">
         <v>404</v>
@@ -36103,7 +36106,7 @@
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="31" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>404</v>
@@ -36157,7 +36160,7 @@
     </row>
     <row r="12" spans="1:19" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="31" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>404</v>
@@ -36211,7 +36214,7 @@
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="112" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="B13" s="113" t="s">
         <v>404</v>
@@ -36265,7 +36268,7 @@
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="31" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="B14" s="32" t="s">
         <v>404</v>
@@ -36319,7 +36322,7 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" s="31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B15" s="32" t="s">
         <v>404</v>
@@ -36376,7 +36379,7 @@
     </row>
     <row r="16" spans="1:19" s="117" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="31" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B16" s="32" t="s">
         <v>404</v>
@@ -36430,7 +36433,7 @@
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" s="31" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B17" s="32" t="s">
         <v>404</v>
@@ -36484,7 +36487,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="31" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="B18" s="32" t="s">
         <v>404</v>
@@ -36538,7 +36541,7 @@
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" s="31" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B19" s="32" t="s">
         <v>404</v>
@@ -36592,7 +36595,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="125" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="B20" s="32" t="s">
         <v>404</v>
@@ -36646,43 +36649,43 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="125" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D21" s="102"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="125" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D22" s="102"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="125" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="D23" s="102"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="125" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D24" s="102"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" s="125" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D25" s="102"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="125" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="D26" s="102"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="125" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="D27" s="102"/>
     </row>
@@ -37081,22 +37084,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="223" t="s">
+      <c r="A1" s="224" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="223"/>
-      <c r="C1" s="223"/>
-      <c r="D1" s="223"/>
-      <c r="E1" s="223"/>
-      <c r="F1" s="223"/>
+      <c r="B1" s="224"/>
+      <c r="C1" s="224"/>
+      <c r="D1" s="224"/>
+      <c r="E1" s="224"/>
+      <c r="F1" s="224"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="223"/>
-      <c r="B2" s="223"/>
-      <c r="C2" s="223"/>
-      <c r="D2" s="223"/>
-      <c r="E2" s="223"/>
-      <c r="F2" s="223"/>
+      <c r="A2" s="224"/>
+      <c r="B2" s="224"/>
+      <c r="C2" s="224"/>
+      <c r="D2" s="224"/>
+      <c r="E2" s="224"/>
+      <c r="F2" s="224"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -37120,10 +37123,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="166" t="s">
+        <v>534</v>
+      </c>
+      <c r="B4" s="165" t="s">
         <v>535</v>
-      </c>
-      <c r="B4" s="165" t="s">
-        <v>536</v>
       </c>
       <c r="C4" s="201">
         <v>200000</v>
@@ -37144,10 +37147,10 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="166" t="s">
+        <v>536</v>
+      </c>
+      <c r="B5" s="163" t="s">
         <v>537</v>
-      </c>
-      <c r="B5" s="163" t="s">
-        <v>538</v>
       </c>
       <c r="C5" s="201">
         <v>100000</v>
@@ -37168,10 +37171,10 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="166" t="s">
+        <v>538</v>
+      </c>
+      <c r="B6" s="165" t="s">
         <v>539</v>
-      </c>
-      <c r="B6" s="165" t="s">
-        <v>540</v>
       </c>
       <c r="C6" s="201">
         <v>300000</v>
@@ -37195,7 +37198,7 @@
         <v>157</v>
       </c>
       <c r="B7" s="163" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="C7" s="201">
         <v>100000</v>
@@ -37216,10 +37219,10 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="166" t="s">
+        <v>541</v>
+      </c>
+      <c r="B8" s="165" t="s">
         <v>542</v>
-      </c>
-      <c r="B8" s="165" t="s">
-        <v>543</v>
       </c>
       <c r="C8" s="201">
         <v>300000</v>
@@ -37243,7 +37246,7 @@
         <v>435</v>
       </c>
       <c r="B9" s="163" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="C9" s="201">
         <v>100000</v>
@@ -37264,10 +37267,10 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="166" t="s">
+        <v>544</v>
+      </c>
+      <c r="B10" s="165" t="s">
         <v>545</v>
-      </c>
-      <c r="B10" s="165" t="s">
-        <v>546</v>
       </c>
       <c r="C10" s="201">
         <v>100000</v>
@@ -37288,10 +37291,10 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="166" t="s">
+        <v>546</v>
+      </c>
+      <c r="B11" s="163" t="s">
         <v>547</v>
-      </c>
-      <c r="B11" s="163" t="s">
-        <v>548</v>
       </c>
       <c r="C11" s="201">
         <v>200000</v>
@@ -37312,10 +37315,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="166" t="s">
+        <v>548</v>
+      </c>
+      <c r="B12" s="163" t="s">
         <v>549</v>
-      </c>
-      <c r="B12" s="163" t="s">
-        <v>550</v>
       </c>
       <c r="C12" s="201"/>
       <c r="D12" s="200">
@@ -37334,10 +37337,10 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="166" t="s">
+        <v>550</v>
+      </c>
+      <c r="B13" s="165" t="s">
         <v>551</v>
-      </c>
-      <c r="B13" s="165" t="s">
-        <v>552</v>
       </c>
       <c r="C13" s="201"/>
       <c r="D13" s="200">
@@ -37356,10 +37359,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="166" t="s">
+        <v>552</v>
+      </c>
+      <c r="B14" s="163" t="s">
         <v>553</v>
-      </c>
-      <c r="B14" s="163" t="s">
-        <v>554</v>
       </c>
       <c r="C14" s="201">
         <v>300000</v>
@@ -37398,7 +37401,7 @@
         <v>-30000</v>
       </c>
       <c r="G15" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="18" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>